<commit_message>
Changes to morbidity & co
</commit_message>
<xml_diff>
--- a/import/raw_data/iiasa/monetisation_factors_updated.xlsx
+++ b/import/raw_data/iiasa/monetisation_factors_updated.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="IIASA_Monetization_MORB-2024-08" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="IIASA_Monetization_MORB-2024-12" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Romania</t>
   </si>
   <si>
-    <t xml:space="preserve">Slovakia</t>
+    <t xml:space="preserve">Slovak Republic</t>
   </si>
   <si>
     <t xml:space="preserve">Slovenia</t>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Sweden</t>
   </si>
   <si>
-    <t xml:space="preserve">European Union27</t>
+    <t xml:space="preserve">EU27</t>
   </si>
 </sst>
 </file>
@@ -325,8 +325,8 @@
   </sheetPr>
   <dimension ref="A1:D617"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A88" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q14" activeCellId="1" sqref="A508:A529 Q14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -460,7 +460,7 @@
         <v>2035</v>
       </c>
       <c r="D9" s="0" t="n">
-        <v>7483.35289156306</v>
+        <v>7401.70179917795</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,7 +474,7 @@
         <v>2040</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>7904.38282014508</v>
+        <v>7750.37653443357</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -488,7 +488,7 @@
         <v>2045</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>8351.54560523393</v>
+        <v>8117.86117015012</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,7 +502,7 @@
         <v>2050</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>8788.42262981616</v>
+        <v>8494.36137078821</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,7 +614,7 @@
         <v>2035</v>
       </c>
       <c r="D20" s="0" t="n">
-        <v>236.420607391115</v>
+        <v>233.841014909568</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,7 +628,7 @@
         <v>2040</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>249.722151884282</v>
+        <v>244.856651066993</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,7 +642,7 @@
         <v>2045</v>
       </c>
       <c r="D22" s="0" t="n">
-        <v>263.849308358835</v>
+        <v>256.466545995369</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,7 +656,7 @@
         <v>2050</v>
       </c>
       <c r="D23" s="0" t="n">
-        <v>277.651508121912</v>
+        <v>268.361268509136</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,7 +768,7 @@
         <v>2035</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>6627.20961693168</v>
+        <v>6334.28581675077</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,7 +782,7 @@
         <v>2040</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>7067.09353398307</v>
+        <v>6522.12183383098</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,7 +796,7 @@
         <v>2045</v>
       </c>
       <c r="D33" s="0" t="n">
-        <v>7506.71224897176</v>
+        <v>6731.10905669204</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +810,7 @@
         <v>2050</v>
       </c>
       <c r="D34" s="0" t="n">
-        <v>7941.13837584935</v>
+        <v>6950.42593620251</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -922,7 +922,7 @@
         <v>2035</v>
       </c>
       <c r="D42" s="0" t="n">
-        <v>233.746978670223</v>
+        <v>223.415322176673</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -936,7 +936,7 @@
         <v>2040</v>
       </c>
       <c r="D43" s="0" t="n">
-        <v>249.26203591448</v>
+        <v>230.040448589722</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,7 +950,7 @@
         <v>2045</v>
       </c>
       <c r="D44" s="0" t="n">
-        <v>264.767739270076</v>
+        <v>237.411594931563</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -964,7 +964,7 @@
         <v>2050</v>
       </c>
       <c r="D45" s="0" t="n">
-        <v>280.090295893848</v>
+        <v>245.147076517354</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,7 +1076,7 @@
         <v>2035</v>
       </c>
       <c r="D53" s="0" t="n">
-        <v>2733.0757204713</v>
+        <v>2594.44198028921</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1090,7 @@
         <v>2040</v>
       </c>
       <c r="D54" s="0" t="n">
-        <v>3017.16552781967</v>
+        <v>2814.2917899465</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1104,7 +1104,7 @@
         <v>2045</v>
       </c>
       <c r="D55" s="0" t="n">
-        <v>3278.47163701345</v>
+        <v>3033.66089949598</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1118,7 @@
         <v>2050</v>
       </c>
       <c r="D56" s="0" t="n">
-        <v>3526.57713994875</v>
+        <v>3250.80446037656</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1230,7 +1230,7 @@
         <v>2035</v>
       </c>
       <c r="D64" s="0" t="n">
-        <v>120.604606632457</v>
+        <v>114.487005288516</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,7 +1244,7 @@
         <v>2040</v>
       </c>
       <c r="D65" s="0" t="n">
-        <v>133.140863570714</v>
+        <v>124.188492742133</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1258,7 +1258,7 @@
         <v>2045</v>
       </c>
       <c r="D66" s="0" t="n">
-        <v>144.671726134793</v>
+        <v>133.868767959669</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,7 +1272,7 @@
         <v>2050</v>
       </c>
       <c r="D67" s="0" t="n">
-        <v>155.620075044679</v>
+        <v>143.450834620543</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1384,7 +1384,7 @@
         <v>2035</v>
       </c>
       <c r="D75" s="0" t="n">
-        <v>2992.69839856996</v>
+        <v>2907.77066500523</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,7 +1398,7 @@
         <v>2040</v>
       </c>
       <c r="D76" s="0" t="n">
-        <v>3183.36531507664</v>
+        <v>3132.49707297846</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1412,7 +1412,7 @@
         <v>2045</v>
       </c>
       <c r="D77" s="0" t="n">
-        <v>3362.51243658504</v>
+        <v>3359.33903217587</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,7 +1426,7 @@
         <v>2050</v>
       </c>
       <c r="D78" s="0" t="n">
-        <v>3533.30558893899</v>
+        <v>3580.19777446808</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,7 +1538,7 @@
         <v>2035</v>
       </c>
       <c r="D86" s="0" t="n">
-        <v>132.201645204161</v>
+        <v>128.449985462544</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,7 +1552,7 @@
         <v>2040</v>
       </c>
       <c r="D87" s="0" t="n">
-        <v>140.624304854808</v>
+        <v>138.377213969459</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1566,7 +1566,7 @@
         <v>2045</v>
       </c>
       <c r="D88" s="0" t="n">
-        <v>148.538080666068</v>
+        <v>148.397896381547</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,7 +1580,7 @@
         <v>2050</v>
       </c>
       <c r="D89" s="0" t="n">
-        <v>156.082822141382</v>
+        <v>158.154271799365</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1692,7 @@
         <v>2035</v>
       </c>
       <c r="D97" s="0" t="n">
-        <v>2229.64404857662</v>
+        <v>2213.71242959498</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,7 +1706,7 @@
         <v>2040</v>
       </c>
       <c r="D98" s="0" t="n">
-        <v>2348.89920870986</v>
+        <v>2403.59491631972</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,7 +1720,7 @@
         <v>2045</v>
       </c>
       <c r="D99" s="0" t="n">
-        <v>2471.12406654209</v>
+        <v>2621.68911999403</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +1734,7 @@
         <v>2050</v>
       </c>
       <c r="D100" s="0" t="n">
-        <v>2592.45419163659</v>
+        <v>2853.50290034393</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1846,7 +1846,7 @@
         <v>2035</v>
       </c>
       <c r="D108" s="0" t="n">
-        <v>130.586124374424</v>
+        <v>129.653038943523</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1860,7 +1860,7 @@
         <v>2040</v>
       </c>
       <c r="D109" s="0" t="n">
-        <v>137.570678336476</v>
+        <v>140.774104677666</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,7 +1874,7 @@
         <v>2045</v>
       </c>
       <c r="D110" s="0" t="n">
-        <v>144.729161995209</v>
+        <v>153.54747844759</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,7 +1888,7 @@
         <v>2050</v>
       </c>
       <c r="D111" s="0" t="n">
-        <v>151.835242813835</v>
+        <v>167.124382425515</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2000,7 +2000,7 @@
         <v>2035</v>
       </c>
       <c r="D119" s="0" t="n">
-        <v>4630.56768400838</v>
+        <v>4462.29556520074</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,7 +2014,7 @@
         <v>2040</v>
       </c>
       <c r="D120" s="0" t="n">
-        <v>5059.67311507721</v>
+        <v>4666.64179327397</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,7 +2028,7 @@
         <v>2045</v>
       </c>
       <c r="D121" s="0" t="n">
-        <v>5438.42737090961</v>
+        <v>4863.63015284799</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2042,7 @@
         <v>2050</v>
       </c>
       <c r="D122" s="0" t="n">
-        <v>5822.10094718396</v>
+        <v>5058.29457426686</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2154,7 +2154,7 @@
         <v>2035</v>
       </c>
       <c r="D130" s="0" t="n">
-        <v>189.342762424148</v>
+        <v>182.462157282788</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2168,7 +2168,7 @@
         <v>2040</v>
       </c>
       <c r="D131" s="0" t="n">
-        <v>206.888776916143</v>
+        <v>190.817823791661</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2182,7 +2182,7 @@
         <v>2045</v>
       </c>
       <c r="D132" s="0" t="n">
-        <v>222.375944359322</v>
+        <v>198.872628885204</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2196,7 @@
         <v>2050</v>
       </c>
       <c r="D133" s="0" t="n">
-        <v>238.064261593474</v>
+        <v>206.832408724821</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2308,7 +2308,7 @@
         <v>2035</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>6394.03257743033</v>
+        <v>6390.14526995917</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2322,7 +2322,7 @@
         <v>2040</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>6715.82752028483</v>
+        <v>6679.71004299064</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2336,7 +2336,7 @@
         <v>2045</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>7105.61172867827</v>
+        <v>7035.47619255911</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2350,7 @@
         <v>2050</v>
       </c>
       <c r="D144" s="0" t="n">
-        <v>7537.82806122436</v>
+        <v>7440.97428236703</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2462,7 +2462,7 @@
         <v>2035</v>
       </c>
       <c r="D152" s="0" t="n">
-        <v>241.746216729663</v>
+        <v>241.599245023929</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2476,7 @@
         <v>2040</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>253.912671788463</v>
+        <v>252.547138631108</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,7 +2490,7 @@
         <v>2045</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>268.649671730048</v>
+        <v>265.997980436675</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2504,7 +2504,7 @@
         <v>2050</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>284.990949622595</v>
+        <v>281.329092362533</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2616,7 +2616,7 @@
         <v>2035</v>
       </c>
       <c r="D163" s="0" t="n">
-        <v>4525.06054468591</v>
+        <v>4462.85263787801</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2630,7 +2630,7 @@
         <v>2040</v>
       </c>
       <c r="D164" s="0" t="n">
-        <v>4987.67486868578</v>
+        <v>4761.3444357895</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2644,7 +2644,7 @@
         <v>2045</v>
       </c>
       <c r="D165" s="0" t="n">
-        <v>5431.57926072162</v>
+        <v>5011.32865364286</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2658,7 +2658,7 @@
         <v>2050</v>
       </c>
       <c r="D166" s="0" t="n">
-        <v>5838.54761972776</v>
+        <v>5241.6331680454</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2770,7 +2770,7 @@
         <v>2035</v>
       </c>
       <c r="D174" s="0" t="n">
-        <v>221.097256731475</v>
+        <v>218.057739932438</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2784,7 +2784,7 @@
         <v>2040</v>
       </c>
       <c r="D175" s="0" t="n">
-        <v>243.700878705368</v>
+        <v>232.642233780278</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2798,7 +2798,7 @@
         <v>2045</v>
       </c>
       <c r="D176" s="0" t="n">
-        <v>265.390321832364</v>
+        <v>244.856617267025</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2812,7 +2812,7 @@
         <v>2050</v>
       </c>
       <c r="D177" s="0" t="n">
-        <v>285.275047542484</v>
+        <v>256.109438272276</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2924,7 +2924,7 @@
         <v>2035</v>
       </c>
       <c r="D185" s="0" t="n">
-        <v>5788.19730176309</v>
+        <v>5725.40414390988</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,7 +2938,7 @@
         <v>2040</v>
       </c>
       <c r="D186" s="0" t="n">
-        <v>6124.15397012348</v>
+        <v>5968.36589108979</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2952,7 +2952,7 @@
         <v>2045</v>
       </c>
       <c r="D187" s="0" t="n">
-        <v>6460.52868826475</v>
+        <v>6191.75931779293</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2966,7 +2966,7 @@
         <v>2050</v>
       </c>
       <c r="D188" s="0" t="n">
-        <v>6798.50050740632</v>
+        <v>6397.89330272989</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,7 +3078,7 @@
         <v>2035</v>
       </c>
       <c r="D196" s="0" t="n">
-        <v>227.080545078032</v>
+        <v>224.617065730475</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3092,7 +3092,7 @@
         <v>2040</v>
       </c>
       <c r="D197" s="0" t="n">
-        <v>240.260680342363</v>
+        <v>234.148856563852</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,7 +3106,7 @@
         <v>2045</v>
       </c>
       <c r="D198" s="0" t="n">
-        <v>253.457216390421</v>
+        <v>242.9129498485</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3120,7 +3120,7 @@
         <v>2050</v>
       </c>
       <c r="D199" s="0" t="n">
-        <v>266.716409349912</v>
+        <v>250.99992671163</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,7 +3232,7 @@
         <v>2035</v>
       </c>
       <c r="D207" s="0" t="n">
-        <v>6290.21702892794</v>
+        <v>6146.13482326095</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,7 +3246,7 @@
         <v>2040</v>
       </c>
       <c r="D208" s="0" t="n">
-        <v>6640.93388559467</v>
+        <v>6347.55080081073</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3260,7 +3260,7 @@
         <v>2045</v>
       </c>
       <c r="D209" s="0" t="n">
-        <v>7008.68106667375</v>
+        <v>6571.88538329666</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3274,7 @@
         <v>2050</v>
       </c>
       <c r="D210" s="0" t="n">
-        <v>7374.95924311352</v>
+        <v>6801.02317712125</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3386,7 +3386,7 @@
         <v>2035</v>
       </c>
       <c r="D218" s="0" t="n">
-        <v>217.71851240399</v>
+        <v>212.731504270974</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3400,7 +3400,7 @@
         <v>2040</v>
       </c>
       <c r="D219" s="0" t="n">
-        <v>229.857609029325</v>
+        <v>219.702962776278</v>
       </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3414,7 +3414,7 @@
         <v>2045</v>
       </c>
       <c r="D220" s="0" t="n">
-        <v>242.586163360135</v>
+        <v>227.467685575983</v>
       </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,7 +3428,7 @@
         <v>2050</v>
       </c>
       <c r="D221" s="0" t="n">
-        <v>255.263872147252</v>
+        <v>235.398658287671</v>
       </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3540,7 +3540,7 @@
         <v>2035</v>
       </c>
       <c r="D229" s="0" t="n">
-        <v>6821.94922147814</v>
+        <v>6818.25110389931</v>
       </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3554,7 +3554,7 @@
         <v>2040</v>
       </c>
       <c r="D230" s="0" t="n">
-        <v>7213.93339861845</v>
+        <v>7147.48896483598</v>
       </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3568,7 +3568,7 @@
         <v>2045</v>
       </c>
       <c r="D231" s="0" t="n">
-        <v>7625.75712427626</v>
+        <v>7526.23655995805</v>
       </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3582,7 +3582,7 @@
         <v>2050</v>
       </c>
       <c r="D232" s="0" t="n">
-        <v>8035.91815982707</v>
+        <v>7931.33236476866</v>
       </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3694,7 +3694,7 @@
         <v>2035</v>
       </c>
       <c r="D240" s="0" t="n">
-        <v>223.119813587474</v>
+        <v>222.998862334684</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3708,7 +3708,7 @@
         <v>2040</v>
       </c>
       <c r="D241" s="0" t="n">
-        <v>235.940113723604</v>
+        <v>233.766970946054</v>
       </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3722,7 +3722,7 @@
         <v>2045</v>
       </c>
       <c r="D242" s="0" t="n">
-        <v>249.409289455722</v>
+        <v>246.154353214201</v>
       </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3736,7 +3736,7 @@
         <v>2050</v>
       </c>
       <c r="D243" s="0" t="n">
-        <v>262.824084966778</v>
+        <v>259.403484440486</v>
       </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3848,7 +3848,7 @@
         <v>2035</v>
       </c>
       <c r="D251" s="0" t="n">
-        <v>4937.20938488987</v>
+        <v>4725.73957989942</v>
       </c>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3862,7 +3862,7 @@
         <v>2040</v>
       </c>
       <c r="D252" s="0" t="n">
-        <v>5310.85597745986</v>
+        <v>4969.76518972304</v>
       </c>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3876,7 +3876,7 @@
         <v>2045</v>
       </c>
       <c r="D253" s="0" t="n">
-        <v>5692.74016521045</v>
+        <v>5228.75778757254</v>
       </c>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3890,7 +3890,7 @@
         <v>2050</v>
       </c>
       <c r="D254" s="0" t="n">
-        <v>6104.38928978339</v>
+        <v>5502.0975212717</v>
       </c>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4002,7 +4002,7 @@
         <v>2035</v>
       </c>
       <c r="D262" s="0" t="n">
-        <v>191.526500645747</v>
+        <v>183.323066562919</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4016,7 +4016,7 @@
         <v>2040</v>
       </c>
       <c r="D263" s="0" t="n">
-        <v>206.02117137455</v>
+        <v>192.789420422754</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4030,7 +4030,7 @@
         <v>2045</v>
       </c>
       <c r="D264" s="0" t="n">
-        <v>220.835398690017</v>
+        <v>202.836380576212</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4044,7 +4044,7 @@
         <v>2050</v>
       </c>
       <c r="D265" s="0" t="n">
-        <v>236.80428114508</v>
+        <v>213.439901432155</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4156,7 +4156,7 @@
         <v>2035</v>
       </c>
       <c r="D273" s="0" t="n">
-        <v>3917.91790700629</v>
+        <v>3855.57438057022</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4170,7 +4170,7 @@
         <v>2040</v>
       </c>
       <c r="D274" s="0" t="n">
-        <v>4275.60536666305</v>
+        <v>4089.15556401581</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4184,7 +4184,7 @@
         <v>2045</v>
       </c>
       <c r="D275" s="0" t="n">
-        <v>4644.01164166216</v>
+        <v>4294.87339356281</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4198,7 +4198,7 @@
         <v>2050</v>
       </c>
       <c r="D276" s="0" t="n">
-        <v>5035.18818605837</v>
+        <v>4537.59171357401</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4310,7 +4310,7 @@
         <v>2035</v>
       </c>
       <c r="D284" s="0" t="n">
-        <v>189.05730347133</v>
+        <v>186.048945645399</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4324,7 +4324,7 @@
         <v>2040</v>
       </c>
       <c r="D285" s="0" t="n">
-        <v>206.317345211175</v>
+        <v>197.320296840608</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4338,7 +4338,7 @@
         <v>2045</v>
       </c>
       <c r="D286" s="0" t="n">
-        <v>224.09461839209</v>
+        <v>207.247114873364</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4352,7 +4352,7 @@
         <v>2050</v>
       </c>
       <c r="D287" s="0" t="n">
-        <v>242.970660315411</v>
+        <v>218.959374337083</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4464,7 +4464,7 @@
         <v>2035</v>
       </c>
       <c r="D295" s="0" t="n">
-        <v>7102.61618012035</v>
+        <v>6978.3845425804</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4478,7 +4478,7 @@
         <v>2040</v>
       </c>
       <c r="D296" s="0" t="n">
-        <v>7437.74995723647</v>
+        <v>7201.98011483446</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4492,7 +4492,7 @@
         <v>2045</v>
       </c>
       <c r="D297" s="0" t="n">
-        <v>7747.58599116212</v>
+        <v>7400.33009284948</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +4506,7 @@
         <v>2050</v>
       </c>
       <c r="D298" s="0" t="n">
-        <v>8074.29773622953</v>
+        <v>7605.77451459896</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4618,7 +4618,7 @@
         <v>2035</v>
       </c>
       <c r="D306" s="0" t="n">
-        <v>257.397112017744</v>
+        <v>252.89498717908</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4632,7 +4632,7 @@
         <v>2040</v>
       </c>
       <c r="D307" s="0" t="n">
-        <v>269.542279964554</v>
+        <v>260.998037252268</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4646,7 +4646,7 @@
         <v>2045</v>
       </c>
       <c r="D308" s="0" t="n">
-        <v>280.770663747238</v>
+        <v>268.186193026861</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4660,7 +4660,7 @@
         <v>2050</v>
       </c>
       <c r="D309" s="0" t="n">
-        <v>292.610619266445</v>
+        <v>275.631449745995</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4772,7 +4772,7 @@
         <v>2035</v>
       </c>
       <c r="D317" s="0" t="n">
-        <v>4996.54698328811</v>
+        <v>4890.45517650176</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4786,7 +4786,7 @@
         <v>2040</v>
       </c>
       <c r="D318" s="0" t="n">
-        <v>5252.79115609466</v>
+        <v>5051.37554195966</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4800,7 +4800,7 @@
         <v>2045</v>
       </c>
       <c r="D319" s="0" t="n">
-        <v>5540.65487365029</v>
+        <v>5235.69586486472</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4814,7 +4814,7 @@
         <v>2050</v>
       </c>
       <c r="D320" s="0" t="n">
-        <v>5866.01105174487</v>
+        <v>5503.20176627188</v>
       </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4926,7 +4926,7 @@
         <v>2035</v>
       </c>
       <c r="D328" s="0" t="n">
-        <v>207.983442916707</v>
+        <v>203.567325282973</v>
       </c>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4940,7 +4940,7 @@
         <v>2040</v>
       </c>
       <c r="D329" s="0" t="n">
-        <v>218.649718139557</v>
+        <v>210.265705535434</v>
       </c>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4954,7 +4954,7 @@
         <v>2045</v>
       </c>
       <c r="D330" s="0" t="n">
-        <v>230.632170674932</v>
+        <v>217.938119201418</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4968,7 +4968,7 @@
         <v>2050</v>
       </c>
       <c r="D331" s="0" t="n">
-        <v>244.175263198762</v>
+        <v>229.073168778914</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5080,7 +5080,7 @@
         <v>2035</v>
       </c>
       <c r="D339" s="0" t="n">
-        <v>3875.38082120197</v>
+        <v>3795.98946857794</v>
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5094,7 +5094,7 @@
         <v>2040</v>
       </c>
       <c r="D340" s="0" t="n">
-        <v>4188.52460363727</v>
+        <v>3968.63674081862</v>
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5108,7 +5108,7 @@
         <v>2045</v>
       </c>
       <c r="D341" s="0" t="n">
-        <v>4489.68587042041</v>
+        <v>4109.12876501424</v>
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5122,7 +5122,7 @@
         <v>2050</v>
       </c>
       <c r="D342" s="0" t="n">
-        <v>4763.57296445306</v>
+        <v>4215.60349700453</v>
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5234,7 +5234,7 @@
         <v>2035</v>
       </c>
       <c r="D350" s="0" t="n">
-        <v>172.196993983458</v>
+        <v>168.669352984838</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5248,7 +5248,7 @@
         <v>2040</v>
       </c>
       <c r="D351" s="0" t="n">
-        <v>186.111089270549</v>
+        <v>176.340687150668</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5262,7 +5262,7 @@
         <v>2045</v>
       </c>
       <c r="D352" s="0" t="n">
-        <v>199.492758643683</v>
+        <v>182.583248942991</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5276,7 +5276,7 @@
         <v>2050</v>
       </c>
       <c r="D353" s="0" t="n">
-        <v>211.662539230216</v>
+        <v>187.31430109756</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5388,7 +5388,7 @@
         <v>2035</v>
       </c>
       <c r="D361" s="0" t="n">
-        <v>3883.38181252819</v>
+        <v>3790.726418341</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5402,7 +5402,7 @@
         <v>2040</v>
       </c>
       <c r="D362" s="0" t="n">
-        <v>4201.27677237312</v>
+        <v>3960.85470383077</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5416,7 +5416,7 @@
         <v>2045</v>
       </c>
       <c r="D363" s="0" t="n">
-        <v>4498.88641569574</v>
+        <v>4129.72833800636</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5430,7 +5430,7 @@
         <v>2050</v>
       </c>
       <c r="D364" s="0" t="n">
-        <v>4748.28000463903</v>
+        <v>4273.22909100666</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5542,7 +5542,7 @@
         <v>2035</v>
       </c>
       <c r="D372" s="0" t="n">
-        <v>169.330552227451</v>
+        <v>165.29041663894</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5556,7 +5556,7 @@
         <v>2040</v>
       </c>
       <c r="D373" s="0" t="n">
-        <v>183.192008993614</v>
+        <v>172.708671634767</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5570,7 +5570,7 @@
         <v>2045</v>
       </c>
       <c r="D374" s="0" t="n">
-        <v>196.168947055552</v>
+        <v>180.072218953076</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5584,7 +5584,7 @@
         <v>2050</v>
       </c>
       <c r="D375" s="0" t="n">
-        <v>207.043477600427</v>
+        <v>186.329409959174</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5696,7 +5696,7 @@
         <v>2035</v>
       </c>
       <c r="D383" s="0" t="n">
-        <v>10196.5851544188</v>
+        <v>10362.5894247709</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5710,7 +5710,7 @@
         <v>2040</v>
       </c>
       <c r="D384" s="0" t="n">
-        <v>10397.9259935659</v>
+        <v>10842.5402890742</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5724,7 +5724,7 @@
         <v>2045</v>
       </c>
       <c r="D385" s="0" t="n">
-        <v>10576.7886953906</v>
+        <v>11339.2547556897</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5738,7 +5738,7 @@
         <v>2050</v>
       </c>
       <c r="D386" s="0" t="n">
-        <v>10749.4646972914</v>
+        <v>11843.2207843933</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5850,7 +5850,7 @@
         <v>2035</v>
       </c>
       <c r="D394" s="0" t="n">
-        <v>430.316060954311</v>
+        <v>437.321769496697</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5864,7 +5864,7 @@
         <v>2040</v>
       </c>
       <c r="D395" s="0" t="n">
-        <v>438.813042590702</v>
+        <v>457.576645246852</v>
       </c>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5878,7 +5878,7 @@
         <v>2045</v>
       </c>
       <c r="D396" s="0" t="n">
-        <v>446.361402373437</v>
+        <v>478.538978170674</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5892,7 +5892,7 @@
         <v>2050</v>
       </c>
       <c r="D397" s="0" t="n">
-        <v>453.648671182946</v>
+        <v>499.807341357201</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6004,7 +6004,7 @@
         <v>2035</v>
       </c>
       <c r="D405" s="0" t="n">
-        <v>4068.22214200033</v>
+        <v>4167.26300650637</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6018,7 +6018,7 @@
         <v>2040</v>
       </c>
       <c r="D406" s="0" t="n">
-        <v>4414.90997609931</v>
+        <v>4605.62548408324</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6032,7 +6032,7 @@
         <v>2045</v>
       </c>
       <c r="D407" s="0" t="n">
-        <v>4736.3421083952</v>
+        <v>4990.09362021083</v>
       </c>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6046,7 +6046,7 @@
         <v>2050</v>
       </c>
       <c r="D408" s="0" t="n">
-        <v>5034.26487158461</v>
+        <v>5311.91660182232</v>
       </c>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6158,7 +6158,7 @@
         <v>2035</v>
       </c>
       <c r="D416" s="0" t="n">
-        <v>168.752048888197</v>
+        <v>172.860317371499</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6172,7 +6172,7 @@
         <v>2040</v>
       </c>
       <c r="D417" s="0" t="n">
-        <v>183.132847253364</v>
+        <v>191.04382939831</v>
       </c>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6186,7 +6186,7 @@
         <v>2045</v>
       </c>
       <c r="D418" s="0" t="n">
-        <v>196.466025484571</v>
+        <v>206.991775070681</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6200,7 +6200,7 @@
         <v>2050</v>
       </c>
       <c r="D419" s="0" t="n">
-        <v>208.824022404062</v>
+        <v>220.341165942327</v>
       </c>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6312,7 +6312,7 @@
         <v>2035</v>
       </c>
       <c r="D427" s="0" t="n">
-        <v>8169.16117335314</v>
+        <v>7937.31144252665</v>
       </c>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6326,7 +6326,7 @@
         <v>2040</v>
       </c>
       <c r="D428" s="0" t="n">
-        <v>8627.158602042</v>
+        <v>8238.2168146258</v>
       </c>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6340,7 +6340,7 @@
         <v>2045</v>
       </c>
       <c r="D429" s="0" t="n">
-        <v>9145.61447273176</v>
+        <v>8670.06778343742</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6354,7 +6354,7 @@
         <v>2050</v>
       </c>
       <c r="D430" s="0" t="n">
-        <v>9681.17942036501</v>
+        <v>9158.83695153264</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6466,7 +6466,7 @@
         <v>2035</v>
       </c>
       <c r="D438" s="0" t="n">
-        <v>247.559928572923</v>
+        <v>240.533906979631</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6480,7 +6480,7 @@
         <v>2040</v>
       </c>
       <c r="D439" s="0" t="n">
-        <v>261.439176188043</v>
+        <v>249.65260482918</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6494,7 +6494,7 @@
         <v>2045</v>
       </c>
       <c r="D440" s="0" t="n">
-        <v>277.150568776896</v>
+        <v>262.739504784328</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6508,7 +6508,7 @@
         <v>2050</v>
       </c>
       <c r="D441" s="0" t="n">
-        <v>293.380438327607</v>
+        <v>277.551265474885</v>
       </c>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6620,7 +6620,7 @@
         <v>2035</v>
       </c>
       <c r="D449" s="0" t="n">
-        <v>3564.53344589617</v>
+        <v>3566.9477094201</v>
       </c>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6634,7 +6634,7 @@
         <v>2040</v>
       </c>
       <c r="D450" s="0" t="n">
-        <v>3847.98942051923</v>
+        <v>3795.80972604391</v>
       </c>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6648,7 +6648,7 @@
         <v>2045</v>
       </c>
       <c r="D451" s="0" t="n">
-        <v>4101.18637302625</v>
+        <v>3985.21206908664</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6662,7 +6662,7 @@
         <v>2050</v>
       </c>
       <c r="D452" s="0" t="n">
-        <v>4328.02818195267</v>
+        <v>4138.40598610248</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6774,7 +6774,7 @@
         <v>2035</v>
       </c>
       <c r="D460" s="0" t="n">
-        <v>172.748163845131</v>
+        <v>172.865166419838</v>
       </c>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6788,7 +6788,7 @@
         <v>2040</v>
       </c>
       <c r="D461" s="0" t="n">
-        <v>186.485305013898</v>
+        <v>183.95651785355</v>
       </c>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6802,7 +6802,7 @@
         <v>2045</v>
       </c>
       <c r="D462" s="0" t="n">
-        <v>198.756001670463</v>
+        <v>193.135533139903</v>
       </c>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6816,7 +6816,7 @@
         <v>2050</v>
       </c>
       <c r="D463" s="0" t="n">
-        <v>209.749447676829</v>
+        <v>200.5597776528</v>
       </c>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6928,7 +6928,7 @@
         <v>2035</v>
       </c>
       <c r="D471" s="0" t="n">
-        <v>4598.70652116012</v>
+        <v>4485.57187862296</v>
       </c>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6942,7 +6942,7 @@
         <v>2040</v>
       </c>
       <c r="D472" s="0" t="n">
-        <v>4879.6082338303</v>
+        <v>4693.87459643071</v>
       </c>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6956,7 +6956,7 @@
         <v>2045</v>
       </c>
       <c r="D473" s="0" t="n">
-        <v>5184.1298341721</v>
+        <v>4948.46779775475</v>
       </c>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6970,7 +6970,7 @@
         <v>2050</v>
       </c>
       <c r="D474" s="0" t="n">
-        <v>5528.51454772506</v>
+        <v>5259.0795288303</v>
       </c>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7082,7 +7082,7 @@
         <v>2035</v>
       </c>
       <c r="D482" s="0" t="n">
-        <v>177.731232376954</v>
+        <v>173.358794312004</v>
       </c>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7096,7 +7096,7 @@
         <v>2040</v>
       </c>
       <c r="D483" s="0" t="n">
-        <v>188.587547590797</v>
+        <v>181.409296898566</v>
       </c>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7110,7 +7110,7 @@
         <v>2045</v>
       </c>
       <c r="D484" s="0" t="n">
-        <v>200.356726394688</v>
+        <v>191.24883834743</v>
       </c>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7124,7 +7124,7 @@
         <v>2050</v>
       </c>
       <c r="D485" s="0" t="n">
-        <v>213.666538462476</v>
+        <v>203.253389083769</v>
       </c>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7236,7 +7236,7 @@
         <v>2035</v>
       </c>
       <c r="D493" s="0" t="n">
-        <v>2160.21587835851</v>
+        <v>2131.25695831864</v>
       </c>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7250,7 +7250,7 @@
         <v>2040</v>
       </c>
       <c r="D494" s="0" t="n">
-        <v>2358.19486872886</v>
+        <v>2277.41785917047</v>
       </c>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7264,7 +7264,7 @@
         <v>2045</v>
       </c>
       <c r="D495" s="0" t="n">
-        <v>2551.46909187008</v>
+        <v>2413.54257069073</v>
       </c>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7278,7 +7278,7 @@
         <v>2050</v>
       </c>
       <c r="D496" s="0" t="n">
-        <v>2752.7117475075</v>
+        <v>2559.11166278944</v>
       </c>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7390,7 +7390,7 @@
         <v>2035</v>
       </c>
       <c r="D504" s="0" t="n">
-        <v>116.616795238067</v>
+        <v>115.053480903404</v>
       </c>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7404,7 +7404,7 @@
         <v>2040</v>
       </c>
       <c r="D505" s="0" t="n">
-        <v>127.304465675432</v>
+        <v>122.943810762196</v>
       </c>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7418,7 +7418,7 @@
         <v>2045</v>
       </c>
       <c r="D506" s="0" t="n">
-        <v>137.738154609328</v>
+        <v>130.292348364031</v>
       </c>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7432,7 +7432,7 @@
         <v>2050</v>
       </c>
       <c r="D507" s="0" t="n">
-        <v>148.602010301133</v>
+        <v>138.150730100937</v>
       </c>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7544,7 +7544,7 @@
         <v>2035</v>
       </c>
       <c r="D515" s="0" t="n">
-        <v>4789.87305276691</v>
+        <v>4648.06196904372</v>
       </c>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7558,7 +7558,7 @@
         <v>2040</v>
       </c>
       <c r="D516" s="0" t="n">
-        <v>5210.2040211713</v>
+        <v>4876.98257933277</v>
       </c>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7572,7 +7572,7 @@
         <v>2045</v>
       </c>
       <c r="D517" s="0" t="n">
-        <v>5604.92486663974</v>
+        <v>5092.38240261625</v>
       </c>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7586,7 +7586,7 @@
         <v>2050</v>
       </c>
       <c r="D518" s="0" t="n">
-        <v>5979.05942176771</v>
+        <v>5289.37717003449</v>
       </c>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7698,7 +7698,7 @@
         <v>2035</v>
       </c>
       <c r="D526" s="0" t="n">
-        <v>198.16279122261</v>
+        <v>192.295896658325</v>
       </c>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7712,7 +7712,7 @@
         <v>2040</v>
       </c>
       <c r="D527" s="0" t="n">
-        <v>215.55238735986</v>
+        <v>201.76661678045</v>
       </c>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7726,7 +7726,7 @@
         <v>2045</v>
       </c>
       <c r="D528" s="0" t="n">
-        <v>231.882462004864</v>
+        <v>210.67796573281</v>
       </c>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7740,7 +7740,7 @@
         <v>2050</v>
       </c>
       <c r="D529" s="0" t="n">
-        <v>247.360857135641</v>
+        <v>218.827875456471</v>
       </c>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7852,7 +7852,7 @@
         <v>2035</v>
       </c>
       <c r="D537" s="0" t="n">
-        <v>5075.24129635572</v>
+        <v>5075.53295974738</v>
       </c>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7866,7 +7866,7 @@
         <v>2040</v>
       </c>
       <c r="D538" s="0" t="n">
-        <v>5432.64918964218</v>
+        <v>5299.57647562033</v>
       </c>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7880,7 +7880,7 @@
         <v>2045</v>
       </c>
       <c r="D539" s="0" t="n">
-        <v>5781.96116832243</v>
+        <v>5484.79498973332</v>
       </c>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7894,7 +7894,7 @@
         <v>2050</v>
       </c>
       <c r="D540" s="0" t="n">
-        <v>6129.00062904981</v>
+        <v>5678.2146052932</v>
       </c>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8006,7 +8006,7 @@
         <v>2035</v>
       </c>
       <c r="D548" s="0" t="n">
-        <v>184.740537613129</v>
+        <v>184.751154261408</v>
       </c>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8020,7 +8020,7 @@
         <v>2040</v>
       </c>
       <c r="D549" s="0" t="n">
-        <v>197.750308478669</v>
+        <v>192.906415687269</v>
       </c>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8034,7 +8034,7 @@
         <v>2045</v>
       </c>
       <c r="D550" s="0" t="n">
-        <v>210.465385253922</v>
+        <v>199.648433627915</v>
       </c>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8048,7 +8048,7 @@
         <v>2050</v>
       </c>
       <c r="D551" s="0" t="n">
-        <v>223.097741590118</v>
+        <v>206.688974496211</v>
       </c>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8160,7 +8160,7 @@
         <v>2035</v>
       </c>
       <c r="D559" s="0" t="n">
-        <v>5600.20757438534</v>
+        <v>5615.04575442799</v>
       </c>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8174,7 +8174,7 @@
         <v>2040</v>
       </c>
       <c r="D560" s="0" t="n">
-        <v>5818.80704458339</v>
+        <v>5830.98585756829</v>
       </c>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8188,7 +8188,7 @@
         <v>2045</v>
       </c>
       <c r="D561" s="0" t="n">
-        <v>6038.58905365601</v>
+        <v>6023.76883108888</v>
       </c>
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8202,7 +8202,7 @@
         <v>2050</v>
       </c>
       <c r="D562" s="0" t="n">
-        <v>6304.38053971947</v>
+        <v>6269.38455384163</v>
       </c>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8314,7 +8314,7 @@
         <v>2035</v>
       </c>
       <c r="D570" s="0" t="n">
-        <v>218.101102384096</v>
+        <v>218.678978004185</v>
       </c>
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8328,7 +8328,7 @@
         <v>2040</v>
       </c>
       <c r="D571" s="0" t="n">
-        <v>226.614498503347</v>
+        <v>227.088804589766</v>
       </c>
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8342,7 +8342,7 @@
         <v>2045</v>
       </c>
       <c r="D572" s="0" t="n">
-        <v>235.173948814114</v>
+        <v>234.596772551174</v>
       </c>
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8356,7 +8356,7 @@
         <v>2050</v>
       </c>
       <c r="D573" s="0" t="n">
-        <v>245.525246573127</v>
+        <v>244.162321539083</v>
       </c>
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8468,7 +8468,7 @@
         <v>2035</v>
       </c>
       <c r="D581" s="0" t="n">
-        <v>6848.01041418371</v>
+        <v>6879.50666555553</v>
       </c>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8482,7 +8482,7 @@
         <v>2040</v>
       </c>
       <c r="D582" s="0" t="n">
-        <v>7210.69698697677</v>
+        <v>7235.72208389398</v>
       </c>
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8496,7 +8496,7 @@
         <v>2045</v>
       </c>
       <c r="D583" s="0" t="n">
-        <v>7583.80029372447</v>
+        <v>7609.16825968377</v>
       </c>
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8510,7 +8510,7 @@
         <v>2050</v>
       </c>
       <c r="D584" s="0" t="n">
-        <v>7937.36684707046</v>
+        <v>7972.94624526395</v>
       </c>
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8622,7 +8622,7 @@
         <v>2035</v>
       </c>
       <c r="D592" s="0" t="n">
-        <v>249.622689253401</v>
+        <v>250.770786071792</v>
       </c>
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8636,7 +8636,7 @@
         <v>2040</v>
       </c>
       <c r="D593" s="0" t="n">
-        <v>262.843287964698</v>
+        <v>263.755499192993</v>
       </c>
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8650,7 +8650,7 @@
         <v>2045</v>
       </c>
       <c r="D594" s="0" t="n">
-        <v>276.443595961717</v>
+        <v>277.368305402949</v>
       </c>
     </row>
     <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8664,7 +8664,7 @@
         <v>2050</v>
       </c>
       <c r="D595" s="0" t="n">
-        <v>289.331753037746</v>
+        <v>290.628688135958</v>
       </c>
     </row>
     <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8874,7 +8874,7 @@
         <v>2035</v>
       </c>
       <c r="D610" s="0" t="n">
-        <v>140299.81477632</v>
+        <v>138362.953570337</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8888,7 +8888,7 @@
         <v>2035</v>
       </c>
       <c r="D611" s="0" t="n">
-        <v>5525.50832483842</v>
+        <v>5450.59728612905</v>
       </c>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8902,7 +8902,7 @@
         <v>2040</v>
       </c>
       <c r="D612" s="0" t="n">
-        <v>149128.051334742</v>
+        <v>145132.503697326</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8916,7 +8916,7 @@
         <v>2040</v>
       </c>
       <c r="D613" s="0" t="n">
-        <v>5879.23724463884</v>
+        <v>5724.38575761084</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8930,7 +8930,7 @@
         <v>2045</v>
       </c>
       <c r="D614" s="0" t="n">
-        <v>157959.3221496</v>
+        <v>152019.242860468</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8944,7 +8944,7 @@
         <v>2045</v>
       </c>
       <c r="D615" s="0" t="n">
-        <v>6231.2134521005</v>
+        <v>6000.05622970914</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8958,7 +8958,7 @@
         <v>2050</v>
       </c>
       <c r="D616" s="0" t="n">
-        <v>166805.462601615</v>
+        <v>159118.43550511</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8972,7 +8972,7 @@
         <v>2050</v>
       </c>
       <c r="D617" s="0" t="n">
-        <v>6582.86813668618</v>
+        <v>6283.02997726185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>